<commit_message>
now prints the gpa requirement for honor classes even if the class is one with the special prerequisite
</commit_message>
<xml_diff>
--- a/prerequisites/trial prereq/execution_files/majors list.xlsx
+++ b/prerequisites/trial prereq/execution_files/majors list.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jcuoncloud-my.sharepoint.com/personal/elettra_scianetti_johncabot_edu/Documents/Documents/advising/prerequisites/trial prereq/execution_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C33D7932-E03C-452A-ACDA-0A7400E5C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B272BBB-3AA6-4179-9EE4-B4987BF50435}"/>
+  <xr:revisionPtr revIDLastSave="811" documentId="13_ncr:1_{C33D7932-E03C-452A-ACDA-0A7400E5C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DDF833F-137E-4010-98C0-1F5FD8C400A2}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="120" windowWidth="14385" windowHeight="15480" xr2:uid="{39B82AA1-F665-4363-970D-8821589D72FA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{39B82AA1-F665-4363-970D-8821589D72FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Majors" sheetId="3" r:id="rId1"/>
     <sheet name="Mj info compact" sheetId="4" r:id="rId2"/>
     <sheet name="Structure" sheetId="1" r:id="rId3"/>
     <sheet name="Esempi" sheetId="2" r:id="rId4"/>
+    <sheet name="PSYCH" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="173">
   <si>
     <t>Major Name</t>
   </si>
@@ -322,14 +323,276 @@
     <t>SOSC</t>
   </si>
   <si>
-    <t>E</t>
+    <t>IT/BUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MKT </t>
+  </si>
+  <si>
+    <t>COR 10</t>
+  </si>
+  <si>
+    <t>COR 11</t>
+  </si>
+  <si>
+    <t>COR 12</t>
+  </si>
+  <si>
+    <t>Four courses at the 300-level or higher to be chosen from: BUS, EC, FIN, LAW, MGT, MKT courses</t>
+  </si>
+  <si>
+    <t>next id</t>
+  </si>
+  <si>
+    <t>Four courses at the 300-level or higher to be chosen from: BUS, EC, FIN, LAW, MGT, MKT courses, MA 209, MA 299 and 400-level MA courses</t>
+  </si>
+  <si>
+    <t>*The two courses must be in the same language, either Latin or Greek</t>
+  </si>
+  <si>
+    <t>In additional it tells you to do two courses in ancient language, problem is that they have to match??</t>
+  </si>
+  <si>
+    <t>ha un altro tipo di checklist prorio</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Six courses at the 200-level or higher to be chosen from HS, LAW, PL or SOSC courses. No more than two courses can be HS ans no more than one can be SOSC. At least four courses must be at the 300-level.</t>
+  </si>
+  <si>
+    <t>Extra info</t>
+  </si>
+  <si>
+    <t>Non ci sono additional requirements</t>
+  </si>
+  <si>
+    <t>Non ci sono additional requirements e nei major electives non c'è nemmeno un corso specifico, sono tutti per concentrations</t>
+  </si>
+  <si>
+    <t>old title row</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Non ci sono additional requirements, inoltre, I major electives sono piuttosto complicati, perché cìé troppa sovrapposizione</t>
+  </si>
+  <si>
+    <t>A maximum of two PL courses can be at 200 level. At least one course must be a 400-level writing intensive senior seminar, for which students with a CUM GPA of 3.5 or above can choose to write a thesis</t>
+  </si>
+  <si>
+    <t>PL 2xx Philosophy of Social Science</t>
+  </si>
+  <si>
+    <t>Writing intensive senior seminar</t>
+  </si>
+  <si>
+    <t>Five additional courses with the PS prefix to be chosen from those not used to fulfil core requirements</t>
+  </si>
+  <si>
+    <t>Two 300 level courses to be chosen from 2 different areas</t>
+  </si>
+  <si>
+    <t>4 LANGUAGES, Non ci sono additional requirements</t>
+  </si>
+  <si>
+    <t>2 LANGUAGES, Non ci sono additional requirements, inoltre, I major electives sono piuttosto complicati, perché cìé troppa sovrapposizione</t>
+  </si>
+  <si>
+    <t>Four courses at the 300-level or higher to be chosen from: BUS, COM, CS, EC, FIN, MGT, MKT courses</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>Four courses at the 300-level or higher to be chosen divided as follow: &gt;Two upper division MKT courses &gt;Two upper division BUS/COM/CMS/DMA/EC/FIN/MGT/MKT or MA 198</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>Five courses to be chosen from : courses not taken in the core, any IT or ITS 300-level and any course from the list of approved substitutes</t>
+  </si>
+  <si>
+    <t>Il problema dei missing additional requirements è che scorrono le lettere</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>other courses in Modern Italian History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOSC/ITS </t>
+  </si>
+  <si>
+    <t>SOSC/ITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUS/ITS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS/ITS </t>
+  </si>
+  <si>
+    <t>HM</t>
+  </si>
+  <si>
+    <r>
+      <t>Five courses to be chosen from : courses not taken in the core</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(si può dire as core courses?)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, any IT or ITS 300-level and any course from the list of approved substitutes</t>
+    </r>
+  </si>
+  <si>
+    <t>any course from the list of approved substitutes</t>
+  </si>
+  <si>
+    <t>ITS</t>
+  </si>
+  <si>
+    <t>Human Communication</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Area / Concentration</t>
+  </si>
+  <si>
+    <t>Cognitive Area</t>
+  </si>
+  <si>
+    <t>PS 312</t>
+  </si>
+  <si>
+    <t>Cognitive Perspectives on Human-Technology Interaction</t>
+  </si>
+  <si>
+    <t>Judgment and Decision Making</t>
+  </si>
+  <si>
+    <t>PS 314</t>
+  </si>
+  <si>
+    <t>Psycholinguistics</t>
+  </si>
+  <si>
+    <t>PS 315</t>
+  </si>
+  <si>
+    <t>Cognitive Area, Psychobiology Area</t>
+  </si>
+  <si>
+    <t>Cognitive Area, Developmental Area</t>
+  </si>
+  <si>
+    <t>PS 321</t>
+  </si>
+  <si>
+    <t>Cognitive Development</t>
+  </si>
+  <si>
+    <t>Developmental Area</t>
+  </si>
+  <si>
+    <t>Adolescent Psychology</t>
+  </si>
+  <si>
+    <t>PS 325</t>
+  </si>
+  <si>
+    <t>Applied Psychology</t>
+  </si>
+  <si>
+    <t>PS 328</t>
+  </si>
+  <si>
+    <t>Educational Psychology</t>
+  </si>
+  <si>
+    <t>Group Dynamics</t>
+  </si>
+  <si>
+    <t>PS 336</t>
+  </si>
+  <si>
+    <t>PS 311</t>
+  </si>
+  <si>
+    <t>Theories of Personality</t>
+  </si>
+  <si>
+    <t>PS 335</t>
+  </si>
+  <si>
+    <t>Sociocultural Area</t>
+  </si>
+  <si>
+    <t>Stereotyping, Prejudice and Discrimination</t>
+  </si>
+  <si>
+    <t>PS 337</t>
+  </si>
+  <si>
+    <t>Industrial/Organizational Psychology</t>
+  </si>
+  <si>
+    <t>PS 340</t>
+  </si>
+  <si>
+    <t>Health Psychology</t>
+  </si>
+  <si>
+    <t>PS 351</t>
+  </si>
+  <si>
+    <t>Clinical Psychology</t>
+  </si>
+  <si>
+    <t>PS 353</t>
+  </si>
+  <si>
+    <t>Abnormal Psychology</t>
+  </si>
+  <si>
+    <t>PS 354</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +621,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +666,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -409,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -436,6 +712,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,6 +795,108 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA6C68A0-87E5-1ED8-AD8A-49287FD1A0E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="1990725"/>
+          <a:ext cx="6457950" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Communications major electives description??</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>7 courses – not taken in the core – to be chosen from 200-level or higher CMS, COM, DMA and DJRN and to be chosen in accordance with the following rules:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Three courses at the 200-level or higher must be chosen from one of these clusters: CMS – DMA – DJRN</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Four courses must be at 300-level or higher (these may also be courses belonging to the cluster)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>No more than two courses other than those coded CMS/COM/DMA/DJRN may be used as major electives</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -815,16 +1200,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701C36C7-83AA-41D8-8B1C-C0D8358D86FD}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F200" sqref="F200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
@@ -836,7 +1221,7 @@
     <col min="12" max="12" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,10 +1235,14 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="F1">
+        <f>'Mj info compact'!F1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -867,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -884,7 +1273,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -901,7 +1290,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -918,7 +1307,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -935,7 +1324,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -952,7 +1341,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -969,7 +1358,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -986,7 +1375,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -1003,7 +1392,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -1020,7 +1409,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -1037,7 +1426,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1054,7 +1443,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1071,7 +1460,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1088,7 +1477,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2014,7 +2403,7 @@
         <v>88</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,103 +3069,389 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>48</v>
+      </c>
+      <c r="B110" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" t="s">
+        <v>99</v>
+      </c>
+      <c r="D110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>56</v>
+      </c>
+      <c r="B111" s="10">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111">
+        <v>110</v>
+      </c>
+      <c r="E111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>57</v>
+      </c>
+      <c r="B112" s="10">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>20</v>
+      </c>
+      <c r="D112">
+        <v>201</v>
+      </c>
+      <c r="E112">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" s="10">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113">
+        <v>202</v>
+      </c>
+      <c r="E113">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>80</v>
+      </c>
+      <c r="B114" s="10">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>16</v>
+      </c>
+      <c r="D114">
+        <v>198</v>
+      </c>
+      <c r="E114">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>81</v>
+      </c>
+      <c r="B115" s="10">
+        <v>1</v>
+      </c>
+      <c r="C115" t="s">
+        <v>16</v>
+      </c>
+      <c r="D115">
+        <v>208</v>
+      </c>
+      <c r="E115">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>62</v>
+      </c>
+      <c r="B116" s="10">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>87</v>
+      </c>
+      <c r="D116">
+        <v>220</v>
+      </c>
+      <c r="E116">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>62</v>
+      </c>
+      <c r="B117" s="10">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>92</v>
+      </c>
+      <c r="D117">
+        <v>303</v>
+      </c>
+      <c r="E117">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>63</v>
+      </c>
+      <c r="B118" s="10">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118">
+        <v>201</v>
+      </c>
+      <c r="E118">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>63</v>
+      </c>
+      <c r="B119" s="10">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>85</v>
+      </c>
+      <c r="D119">
+        <v>201</v>
+      </c>
+      <c r="E119">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>73</v>
+      </c>
+      <c r="B120" s="10">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120">
+        <v>202</v>
+      </c>
+      <c r="E120">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>73</v>
+      </c>
+      <c r="B121" s="10">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>85</v>
+      </c>
+      <c r="D121">
+        <v>202</v>
+      </c>
+      <c r="E121">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>74</v>
+      </c>
+      <c r="B122" s="10">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>21</v>
+      </c>
+      <c r="D122">
+        <v>301</v>
+      </c>
+      <c r="E122">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>75</v>
+      </c>
+      <c r="B123" s="10">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>93</v>
+      </c>
+      <c r="D123">
+        <v>323</v>
+      </c>
+      <c r="E123">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>76</v>
+      </c>
+      <c r="B124" s="10">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>95</v>
+      </c>
+      <c r="D124">
+        <v>301</v>
+      </c>
+      <c r="E124">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>77</v>
+      </c>
+      <c r="B125" s="10">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>94</v>
+      </c>
+      <c r="D125">
+        <v>301</v>
+      </c>
+      <c r="E125">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>78</v>
+      </c>
+      <c r="B126" s="10">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>94</v>
+      </c>
+      <c r="D126">
+        <v>310</v>
+      </c>
+      <c r="E126">
+        <v>310</v>
+      </c>
+    </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="B127" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D127">
-        <v>200</v>
+        <v>330</v>
       </c>
       <c r="E127">
-        <v>1000</v>
+        <v>330</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="B128" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="D128">
-        <v>200</v>
+        <v>330</v>
       </c>
       <c r="E128">
-        <v>1000</v>
+        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B129" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D129">
-        <v>200</v>
+        <v>426</v>
       </c>
       <c r="E129">
-        <v>1000</v>
+        <v>426</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B130" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="D130">
-        <v>200</v>
+        <v>330</v>
       </c>
       <c r="E130">
-        <v>1000</v>
+        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B131" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="D131">
-        <v>200</v>
+        <v>498</v>
       </c>
       <c r="E131">
-        <v>1000</v>
+        <v>498</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B132" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="D132">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E132">
         <v>1000</v>
@@ -2784,16 +3459,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B133" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D133">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E133">
         <v>1000</v>
@@ -2801,16 +3476,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B134" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C134" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D134">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E134">
         <v>1000</v>
@@ -2818,30 +3493,2476 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>59</v>
+      </c>
+      <c r="B135" s="10">
+        <v>4</v>
+      </c>
+      <c r="C135" t="s">
+        <v>22</v>
+      </c>
+      <c r="D135">
+        <v>300</v>
+      </c>
+      <c r="E135">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>59</v>
+      </c>
+      <c r="B136" s="10">
+        <v>4</v>
+      </c>
+      <c r="C136" t="s">
+        <v>23</v>
+      </c>
+      <c r="D136">
+        <v>300</v>
+      </c>
+      <c r="E136">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>59</v>
+      </c>
+      <c r="B137" s="10">
+        <v>4</v>
+      </c>
+      <c r="C137" t="s">
+        <v>24</v>
+      </c>
+      <c r="D137">
+        <v>300</v>
+      </c>
+      <c r="E137">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>31</v>
+      </c>
+      <c r="B138" t="s">
+        <v>13</v>
+      </c>
+      <c r="C138" t="s">
+        <v>101</v>
+      </c>
+      <c r="D138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>56</v>
+      </c>
+      <c r="B139" s="10">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139">
+        <v>110</v>
+      </c>
+      <c r="E139">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>57</v>
+      </c>
+      <c r="B140" s="10">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>16</v>
+      </c>
+      <c r="D140">
+        <v>198</v>
+      </c>
+      <c r="E140">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>79</v>
+      </c>
+      <c r="B141" s="10">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>16</v>
+      </c>
+      <c r="D141">
+        <v>208</v>
+      </c>
+      <c r="E141">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>62</v>
+      </c>
+      <c r="B142" s="10">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>87</v>
+      </c>
+      <c r="D142">
+        <v>220</v>
+      </c>
+      <c r="E142">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>63</v>
+      </c>
+      <c r="B143" s="10">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>20</v>
+      </c>
+      <c r="D143">
+        <v>201</v>
+      </c>
+      <c r="E143">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>73</v>
+      </c>
+      <c r="B144" s="10">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>20</v>
+      </c>
+      <c r="D144">
+        <v>202</v>
+      </c>
+      <c r="E144">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>74</v>
+      </c>
+      <c r="B145" s="10">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
+        <v>21</v>
+      </c>
+      <c r="D145">
+        <v>201</v>
+      </c>
+      <c r="E145">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>74</v>
+      </c>
+      <c r="B146" s="10">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>85</v>
+      </c>
+      <c r="D146">
+        <v>201</v>
+      </c>
+      <c r="E146">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>75</v>
+      </c>
+      <c r="B147" s="10">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s">
+        <v>21</v>
+      </c>
+      <c r="D147">
+        <v>202</v>
+      </c>
+      <c r="E147">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>75</v>
+      </c>
+      <c r="B148" s="10">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s">
+        <v>85</v>
+      </c>
+      <c r="D148">
+        <v>202</v>
+      </c>
+      <c r="E148">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>76</v>
+      </c>
+      <c r="B149" s="10">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>21</v>
+      </c>
+      <c r="D149">
+        <v>301</v>
+      </c>
+      <c r="E149">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>77</v>
+      </c>
+      <c r="B150" s="10">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>93</v>
+      </c>
+      <c r="D150">
+        <v>219</v>
+      </c>
+      <c r="E150">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>78</v>
+      </c>
+      <c r="B151" s="10">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>95</v>
+      </c>
+      <c r="D151">
+        <v>301</v>
+      </c>
+      <c r="E151">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>89</v>
+      </c>
+      <c r="B152" s="10">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>94</v>
+      </c>
+      <c r="D152">
+        <v>301</v>
+      </c>
+      <c r="E152">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>96</v>
+      </c>
+      <c r="B153" s="10">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>94</v>
+      </c>
+      <c r="D153">
+        <v>310</v>
+      </c>
+      <c r="E153">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>97</v>
+      </c>
+      <c r="B154" s="10">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>94</v>
+      </c>
+      <c r="D154">
+        <v>330</v>
+      </c>
+      <c r="E154">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>98</v>
+      </c>
+      <c r="B155" s="10">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>23</v>
+      </c>
+      <c r="D155">
+        <v>498</v>
+      </c>
+      <c r="E155">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>59</v>
+      </c>
+      <c r="B156" s="10">
+        <v>4</v>
+      </c>
+      <c r="C156" t="s">
+        <v>87</v>
+      </c>
+      <c r="D156">
+        <v>300</v>
+      </c>
+      <c r="E156">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>59</v>
+      </c>
+      <c r="B157" s="10">
+        <v>4</v>
+      </c>
+      <c r="C157" t="s">
+        <v>20</v>
+      </c>
+      <c r="D157">
+        <v>300</v>
+      </c>
+      <c r="E157">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>59</v>
+      </c>
+      <c r="B158" s="10">
+        <v>4</v>
+      </c>
+      <c r="C158" t="s">
+        <v>21</v>
+      </c>
+      <c r="D158">
+        <v>300</v>
+      </c>
+      <c r="E158">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>59</v>
+      </c>
+      <c r="B159" s="10">
+        <v>4</v>
+      </c>
+      <c r="C159" t="s">
+        <v>22</v>
+      </c>
+      <c r="D159">
+        <v>300</v>
+      </c>
+      <c r="E159">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>59</v>
+      </c>
+      <c r="B160" s="10">
+        <v>4</v>
+      </c>
+      <c r="C160" t="s">
+        <v>23</v>
+      </c>
+      <c r="D160">
+        <v>300</v>
+      </c>
+      <c r="E160">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>59</v>
+      </c>
+      <c r="B161" s="10">
+        <v>4</v>
+      </c>
+      <c r="C161" t="s">
+        <v>24</v>
+      </c>
+      <c r="D161">
+        <v>300</v>
+      </c>
+      <c r="E161">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>59</v>
+      </c>
+      <c r="B162" s="10">
+        <v>4</v>
+      </c>
+      <c r="C162" t="s">
+        <v>16</v>
+      </c>
+      <c r="D162">
+        <v>209</v>
+      </c>
+      <c r="E162">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>59</v>
+      </c>
+      <c r="B163" s="10">
+        <v>4</v>
+      </c>
+      <c r="C163" t="s">
+        <v>16</v>
+      </c>
+      <c r="D163">
+        <v>299</v>
+      </c>
+      <c r="E163">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>59</v>
+      </c>
+      <c r="B164" s="10">
+        <v>4</v>
+      </c>
+      <c r="C164" t="s">
+        <v>16</v>
+      </c>
+      <c r="D164">
+        <v>400</v>
+      </c>
+      <c r="E164">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>54</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C165" t="s">
+        <v>106</v>
+      </c>
+      <c r="D165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>62</v>
+      </c>
+      <c r="B166" s="10">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>111</v>
+      </c>
+      <c r="D166">
+        <v>210</v>
+      </c>
+      <c r="E166">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>63</v>
+      </c>
+      <c r="B167" s="10">
+        <v>1</v>
+      </c>
+      <c r="C167" t="s">
+        <v>111</v>
+      </c>
+      <c r="D167">
+        <v>211</v>
+      </c>
+      <c r="E167">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>73</v>
+      </c>
+      <c r="B168" s="10">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>25</v>
+      </c>
+      <c r="D168">
+        <v>101</v>
+      </c>
+      <c r="E168">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>74</v>
+      </c>
+      <c r="B169" s="10">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>25</v>
+      </c>
+      <c r="D169">
+        <v>201</v>
+      </c>
+      <c r="E169">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>75</v>
+      </c>
+      <c r="B170" s="10">
+        <v>1</v>
+      </c>
+      <c r="C170" t="s">
+        <v>25</v>
+      </c>
+      <c r="D170">
+        <v>209</v>
+      </c>
+      <c r="E170">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>76</v>
+      </c>
+      <c r="B171" s="10">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>25</v>
+      </c>
+      <c r="D171">
+        <v>210</v>
+      </c>
+      <c r="E171">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>77</v>
+      </c>
+      <c r="B172" s="10">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>25</v>
+      </c>
+      <c r="D172">
+        <v>223</v>
+      </c>
+      <c r="E172">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>78</v>
+      </c>
+      <c r="B173" s="10">
+        <v>1</v>
+      </c>
+      <c r="C173" t="s">
+        <v>25</v>
+      </c>
+      <c r="D173">
+        <v>250</v>
+      </c>
+      <c r="E173">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>89</v>
+      </c>
+      <c r="B174" s="10">
+        <v>1</v>
+      </c>
+      <c r="C174" t="s">
+        <v>25</v>
+      </c>
+      <c r="D174">
+        <v>340</v>
+      </c>
+      <c r="E174">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>96</v>
+      </c>
+      <c r="B175" s="10">
+        <v>1</v>
+      </c>
+      <c r="C175" t="s">
+        <v>25</v>
+      </c>
+      <c r="D175">
+        <v>460</v>
+      </c>
+      <c r="E175">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>97</v>
+      </c>
+      <c r="B176" s="10">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
+        <v>25</v>
+      </c>
+      <c r="D176">
+        <v>480</v>
+      </c>
+      <c r="E176">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>53</v>
+      </c>
+      <c r="B177" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C177" t="s">
+        <v>113</v>
+      </c>
+      <c r="D177">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>62</v>
+      </c>
+      <c r="B178" s="10">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s">
+        <v>25</v>
+      </c>
+      <c r="D178">
+        <v>209</v>
+      </c>
+      <c r="E178">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>63</v>
+      </c>
+      <c r="B179" s="10">
+        <v>1</v>
+      </c>
+      <c r="C179" t="s">
+        <v>25</v>
+      </c>
+      <c r="D179">
+        <v>210</v>
+      </c>
+      <c r="E179">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>73</v>
+      </c>
+      <c r="B180" s="10">
+        <v>1</v>
+      </c>
+      <c r="C180" t="s">
+        <v>25</v>
+      </c>
+      <c r="D180">
+        <v>223</v>
+      </c>
+      <c r="E180">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>74</v>
+      </c>
+      <c r="B181" s="10">
+        <v>1</v>
+      </c>
+      <c r="C181" t="s">
+        <v>25</v>
+      </c>
+      <c r="D181">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>74</v>
+      </c>
+      <c r="B182" s="10">
+        <v>1</v>
+      </c>
+      <c r="C182" t="s">
+        <v>25</v>
+      </c>
+      <c r="D182">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>74</v>
+      </c>
+      <c r="B183" s="10">
+        <v>1</v>
+      </c>
+      <c r="C183" t="s">
+        <v>25</v>
+      </c>
+      <c r="D183" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E183" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F183" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>74</v>
+      </c>
+      <c r="B184" s="10">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s">
+        <v>25</v>
+      </c>
+      <c r="D184">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>75</v>
+      </c>
+      <c r="B185" s="10">
+        <v>1</v>
+      </c>
+      <c r="C185" t="s">
+        <v>25</v>
+      </c>
+      <c r="D185">
+        <v>200</v>
+      </c>
+      <c r="E185">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>59</v>
+      </c>
+      <c r="B186" s="10">
+        <v>1</v>
+      </c>
+      <c r="F186" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>60</v>
       </c>
-      <c r="B135" s="10">
+      <c r="B187" s="10">
         <v>3</v>
       </c>
-      <c r="C135" t="s">
+      <c r="F187" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>60</v>
+      </c>
+      <c r="B188" s="10">
+        <v>3</v>
+      </c>
+      <c r="C188" t="s">
+        <v>25</v>
+      </c>
+      <c r="D188">
+        <v>300</v>
+      </c>
+      <c r="E188">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>61</v>
+      </c>
+      <c r="B189" s="10">
+        <v>2</v>
+      </c>
+      <c r="F189" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>61</v>
+      </c>
+      <c r="B190" s="10">
+        <v>2</v>
+      </c>
+      <c r="C190" t="s">
+        <v>25</v>
+      </c>
+      <c r="D190">
+        <v>200</v>
+      </c>
+      <c r="E190">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>55</v>
+      </c>
+      <c r="B191" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C191" t="s">
+        <v>116</v>
+      </c>
+      <c r="D191">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>62</v>
+      </c>
+      <c r="B192" s="10">
+        <v>1</v>
+      </c>
+      <c r="C192" t="s">
         <v>26</v>
       </c>
-      <c r="D135">
+      <c r="D192">
+        <v>101</v>
+      </c>
+      <c r="E192">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>63</v>
+      </c>
+      <c r="B193" s="10">
+        <v>1</v>
+      </c>
+      <c r="C193" t="s">
+        <v>26</v>
+      </c>
+      <c r="D193">
+        <v>208</v>
+      </c>
+      <c r="E193">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>73</v>
+      </c>
+      <c r="B194" s="10">
+        <v>1</v>
+      </c>
+      <c r="C194" t="s">
+        <v>26</v>
+      </c>
+      <c r="D194">
+        <v>210</v>
+      </c>
+      <c r="E194">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>74</v>
+      </c>
+      <c r="B195" s="10">
+        <v>1</v>
+      </c>
+      <c r="C195" t="s">
+        <v>26</v>
+      </c>
+      <c r="D195">
+        <v>307</v>
+      </c>
+      <c r="E195">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>75</v>
+      </c>
+      <c r="B196" s="10">
+        <v>1</v>
+      </c>
+      <c r="C196" t="s">
+        <v>26</v>
+      </c>
+      <c r="D196">
+        <v>320</v>
+      </c>
+      <c r="E196">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>76</v>
+      </c>
+      <c r="B197" s="10">
+        <v>1</v>
+      </c>
+      <c r="C197" t="s">
+        <v>26</v>
+      </c>
+      <c r="D197">
+        <v>334</v>
+      </c>
+      <c r="E197">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>77</v>
+      </c>
+      <c r="B198" s="10">
+        <v>1</v>
+      </c>
+      <c r="C198" t="s">
+        <v>26</v>
+      </c>
+      <c r="D198">
+        <v>370</v>
+      </c>
+      <c r="E198">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>78</v>
+      </c>
+      <c r="B199" s="10">
+        <v>1</v>
+      </c>
+      <c r="C199" t="s">
+        <v>26</v>
+      </c>
+      <c r="D199">
+        <v>480</v>
+      </c>
+      <c r="E199">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>89</v>
+      </c>
+      <c r="B200" s="10">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
+        <v>26</v>
+      </c>
+      <c r="D200" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E200" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F200" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>96</v>
+      </c>
+      <c r="B201" s="10">
+        <v>1</v>
+      </c>
+      <c r="C201" t="s">
+        <v>26</v>
+      </c>
+      <c r="D201">
+        <v>354</v>
+      </c>
+      <c r="E201">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>96</v>
+      </c>
+      <c r="B202" s="10">
+        <v>1</v>
+      </c>
+      <c r="C202" t="s">
+        <v>26</v>
+      </c>
+      <c r="D202">
+        <v>353</v>
+      </c>
+      <c r="E202">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>96</v>
+      </c>
+      <c r="B203" s="10">
+        <v>1</v>
+      </c>
+      <c r="C203" t="s">
+        <v>26</v>
+      </c>
+      <c r="D203">
+        <v>328</v>
+      </c>
+      <c r="E203">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>96</v>
+      </c>
+      <c r="B204" s="10">
+        <v>1</v>
+      </c>
+      <c r="C204" t="s">
+        <v>26</v>
+      </c>
+      <c r="D204">
+        <v>351</v>
+      </c>
+      <c r="E204">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>96</v>
+      </c>
+      <c r="B205" s="10">
+        <v>1</v>
+      </c>
+      <c r="C205" t="s">
+        <v>26</v>
+      </c>
+      <c r="D205">
+        <v>340</v>
+      </c>
+      <c r="E205">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>59</v>
+      </c>
+      <c r="B206" s="10">
+        <v>5</v>
+      </c>
+      <c r="C206" t="s">
+        <v>26</v>
+      </c>
+      <c r="D206">
         <v>200</v>
       </c>
-      <c r="E135">
-        <v>1000</v>
+      <c r="E206">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>52</v>
+      </c>
+      <c r="B207" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C207" t="s">
+        <v>120</v>
+      </c>
+      <c r="D207">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>56</v>
+      </c>
+      <c r="B208" s="10">
+        <v>1</v>
+      </c>
+      <c r="C208" t="s">
+        <v>21</v>
+      </c>
+      <c r="D208">
+        <v>201</v>
+      </c>
+      <c r="E208">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>56</v>
+      </c>
+      <c r="B209" s="10">
+        <v>1</v>
+      </c>
+      <c r="C209" t="s">
+        <v>85</v>
+      </c>
+      <c r="D209">
+        <v>201</v>
+      </c>
+      <c r="E209">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>57</v>
+      </c>
+      <c r="B210" s="10">
+        <v>1</v>
+      </c>
+      <c r="C210" t="s">
+        <v>21</v>
+      </c>
+      <c r="D210">
+        <v>202</v>
+      </c>
+      <c r="E210">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>57</v>
+      </c>
+      <c r="B211" s="10">
+        <v>1</v>
+      </c>
+      <c r="C211" t="s">
+        <v>85</v>
+      </c>
+      <c r="D211">
+        <v>202</v>
+      </c>
+      <c r="E211">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>79</v>
+      </c>
+      <c r="B212" s="10">
+        <v>1</v>
+      </c>
+      <c r="C212" t="s">
+        <v>16</v>
+      </c>
+      <c r="D212">
+        <v>198</v>
+      </c>
+      <c r="E212">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>80</v>
+      </c>
+      <c r="B213" s="10">
+        <v>1</v>
+      </c>
+      <c r="C213" t="s">
+        <v>16</v>
+      </c>
+      <c r="D213">
+        <v>208</v>
+      </c>
+      <c r="E213">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>81</v>
+      </c>
+      <c r="B214" s="10">
+        <v>1</v>
+      </c>
+      <c r="C214" t="s">
+        <v>16</v>
+      </c>
+      <c r="D214">
+        <v>209</v>
+      </c>
+      <c r="E214">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>62</v>
+      </c>
+      <c r="B215" s="10">
+        <v>1</v>
+      </c>
+      <c r="C215" t="s">
+        <v>87</v>
+      </c>
+      <c r="D215">
+        <v>220</v>
+      </c>
+      <c r="E215">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>63</v>
+      </c>
+      <c r="B216" s="10">
+        <v>1</v>
+      </c>
+      <c r="C216" t="s">
+        <v>20</v>
+      </c>
+      <c r="D216">
+        <v>201</v>
+      </c>
+      <c r="E216">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>73</v>
+      </c>
+      <c r="B217" s="10">
+        <v>1</v>
+      </c>
+      <c r="C217" t="s">
+        <v>20</v>
+      </c>
+      <c r="D217">
+        <v>202</v>
+      </c>
+      <c r="E217">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>74</v>
+      </c>
+      <c r="B218" s="10">
+        <v>1</v>
+      </c>
+      <c r="C218" t="s">
+        <v>21</v>
+      </c>
+      <c r="D218">
+        <v>301</v>
+      </c>
+      <c r="E218">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>75</v>
+      </c>
+      <c r="B219" s="10">
+        <v>1</v>
+      </c>
+      <c r="C219" t="s">
+        <v>24</v>
+      </c>
+      <c r="D219">
+        <v>301</v>
+      </c>
+      <c r="E219">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>76</v>
+      </c>
+      <c r="B220" s="10">
+        <v>1</v>
+      </c>
+      <c r="C220" t="s">
+        <v>24</v>
+      </c>
+      <c r="D220">
+        <v>302</v>
+      </c>
+      <c r="E220">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>76</v>
+      </c>
+      <c r="B221" s="10">
+        <v>1</v>
+      </c>
+      <c r="C221" t="s">
+        <v>24</v>
+      </c>
+      <c r="D221">
+        <v>304</v>
+      </c>
+      <c r="E221">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>77</v>
+      </c>
+      <c r="B222" s="10">
+        <v>1</v>
+      </c>
+      <c r="C222" t="s">
+        <v>24</v>
+      </c>
+      <c r="D222">
+        <v>305</v>
+      </c>
+      <c r="E222">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>78</v>
+      </c>
+      <c r="B223" s="10">
+        <v>1</v>
+      </c>
+      <c r="C223" t="s">
+        <v>24</v>
+      </c>
+      <c r="D223">
+        <v>310</v>
+      </c>
+      <c r="E223">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>89</v>
+      </c>
+      <c r="B224" s="10">
+        <v>1</v>
+      </c>
+      <c r="C224" t="s">
+        <v>24</v>
+      </c>
+      <c r="D224">
+        <v>320</v>
+      </c>
+      <c r="E224">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>96</v>
+      </c>
+      <c r="B225" s="10">
+        <v>1</v>
+      </c>
+      <c r="C225" t="s">
+        <v>24</v>
+      </c>
+      <c r="D225">
+        <v>490</v>
+      </c>
+      <c r="E225">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>59</v>
+      </c>
+      <c r="B226" s="10">
+        <v>4</v>
+      </c>
+      <c r="C226" t="s">
+        <v>87</v>
+      </c>
+      <c r="D226">
+        <v>300</v>
+      </c>
+      <c r="E226">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>59</v>
+      </c>
+      <c r="B227" s="10">
+        <v>4</v>
+      </c>
+      <c r="C227" t="s">
+        <v>121</v>
+      </c>
+      <c r="D227">
+        <v>300</v>
+      </c>
+      <c r="E227">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>59</v>
+      </c>
+      <c r="B228" s="10">
+        <v>4</v>
+      </c>
+      <c r="C228" t="s">
+        <v>15</v>
+      </c>
+      <c r="D228">
+        <v>300</v>
+      </c>
+      <c r="E228">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>59</v>
+      </c>
+      <c r="B229" s="10">
+        <v>4</v>
+      </c>
+      <c r="C229" t="s">
+        <v>20</v>
+      </c>
+      <c r="D229">
+        <v>300</v>
+      </c>
+      <c r="E229">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>59</v>
+      </c>
+      <c r="B230" s="10">
+        <v>4</v>
+      </c>
+      <c r="C230" t="s">
+        <v>21</v>
+      </c>
+      <c r="D230">
+        <v>300</v>
+      </c>
+      <c r="E230">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>59</v>
+      </c>
+      <c r="B231" s="10">
+        <v>4</v>
+      </c>
+      <c r="C231" t="s">
+        <v>23</v>
+      </c>
+      <c r="D231">
+        <v>300</v>
+      </c>
+      <c r="E231">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>59</v>
+      </c>
+      <c r="B232" s="10">
+        <v>4</v>
+      </c>
+      <c r="C232" t="s">
+        <v>24</v>
+      </c>
+      <c r="D232">
+        <v>300</v>
+      </c>
+      <c r="E232">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>51</v>
+      </c>
+      <c r="B233" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C233" t="s">
+        <v>122</v>
+      </c>
+      <c r="D233">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>56</v>
+      </c>
+      <c r="B234" s="10">
+        <v>1</v>
+      </c>
+      <c r="C234" t="s">
+        <v>121</v>
+      </c>
+      <c r="D234">
+        <v>111</v>
+      </c>
+      <c r="E234">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>57</v>
+      </c>
+      <c r="B235" s="10">
+        <v>1</v>
+      </c>
+      <c r="C235" t="s">
+        <v>15</v>
+      </c>
+      <c r="D235">
+        <v>110</v>
+      </c>
+      <c r="E235">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>79</v>
+      </c>
+      <c r="B236" s="10">
+        <v>1</v>
+      </c>
+      <c r="C236" t="s">
+        <v>20</v>
+      </c>
+      <c r="D236">
+        <v>201</v>
+      </c>
+      <c r="E236">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>80</v>
+      </c>
+      <c r="B237" s="10">
+        <v>1</v>
+      </c>
+      <c r="C237" t="s">
+        <v>21</v>
+      </c>
+      <c r="D237">
+        <v>201</v>
+      </c>
+      <c r="E237">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>80</v>
+      </c>
+      <c r="B238" s="10">
+        <v>1</v>
+      </c>
+      <c r="C238" t="s">
+        <v>85</v>
+      </c>
+      <c r="D238">
+        <v>201</v>
+      </c>
+      <c r="E238">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>81</v>
+      </c>
+      <c r="B239" s="10">
+        <v>1</v>
+      </c>
+      <c r="C239" t="s">
+        <v>16</v>
+      </c>
+      <c r="D239">
+        <v>208</v>
+      </c>
+      <c r="E239">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>82</v>
+      </c>
+      <c r="B240" s="10">
+        <v>1</v>
+      </c>
+      <c r="C240" t="s">
+        <v>26</v>
+      </c>
+      <c r="D240">
+        <v>101</v>
+      </c>
+      <c r="E240">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>62</v>
+      </c>
+      <c r="B241" s="10">
+        <v>1</v>
+      </c>
+      <c r="C241" t="s">
+        <v>16</v>
+      </c>
+      <c r="D241">
+        <v>209</v>
+      </c>
+      <c r="E241">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>63</v>
+      </c>
+      <c r="B242" s="10">
+        <v>1</v>
+      </c>
+      <c r="C242" t="s">
+        <v>87</v>
+      </c>
+      <c r="D242">
+        <v>220</v>
+      </c>
+      <c r="E242">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>73</v>
+      </c>
+      <c r="B243" s="10">
+        <v>1</v>
+      </c>
+      <c r="C243" t="s">
+        <v>24</v>
+      </c>
+      <c r="D243">
+        <v>301</v>
+      </c>
+      <c r="E243">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>74</v>
+      </c>
+      <c r="B244" s="10">
+        <v>1</v>
+      </c>
+      <c r="C244" t="s">
+        <v>24</v>
+      </c>
+      <c r="D244">
+        <v>305</v>
+      </c>
+      <c r="E244">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>75</v>
+      </c>
+      <c r="B245" s="10">
+        <v>1</v>
+      </c>
+      <c r="C245" t="s">
+        <v>24</v>
+      </c>
+      <c r="D245">
+        <v>304</v>
+      </c>
+      <c r="E245">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>75</v>
+      </c>
+      <c r="B246" s="10">
+        <v>1</v>
+      </c>
+      <c r="C246" t="s">
+        <v>24</v>
+      </c>
+      <c r="D246">
+        <v>340</v>
+      </c>
+      <c r="E246">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>76</v>
+      </c>
+      <c r="B247" s="10">
+        <v>1</v>
+      </c>
+      <c r="C247" t="s">
+        <v>24</v>
+      </c>
+      <c r="D247">
+        <v>310</v>
+      </c>
+      <c r="E247">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>77</v>
+      </c>
+      <c r="B248" s="10">
+        <v>1</v>
+      </c>
+      <c r="C248" t="s">
+        <v>24</v>
+      </c>
+      <c r="D248">
+        <v>320</v>
+      </c>
+      <c r="E248">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>78</v>
+      </c>
+      <c r="B249" s="10">
+        <v>1</v>
+      </c>
+      <c r="C249" t="s">
+        <v>24</v>
+      </c>
+      <c r="D249">
+        <v>490</v>
+      </c>
+      <c r="E249">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>59</v>
+      </c>
+      <c r="B250" s="10">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>24</v>
+      </c>
+      <c r="D250">
+        <v>300</v>
+      </c>
+      <c r="E250">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>60</v>
+      </c>
+      <c r="B251" s="10">
+        <v>2</v>
+      </c>
+      <c r="C251" t="s">
+        <v>87</v>
+      </c>
+      <c r="D251">
+        <v>300</v>
+      </c>
+      <c r="E251">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>60</v>
+      </c>
+      <c r="B252" s="10">
+        <v>2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>121</v>
+      </c>
+      <c r="D252">
+        <v>300</v>
+      </c>
+      <c r="E252">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>60</v>
+      </c>
+      <c r="B253" s="10">
+        <v>2</v>
+      </c>
+      <c r="C253" t="s">
+        <v>123</v>
+      </c>
+      <c r="D253">
+        <v>300</v>
+      </c>
+      <c r="E253">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>60</v>
+      </c>
+      <c r="B254" s="10">
+        <v>2</v>
+      </c>
+      <c r="C254" t="s">
+        <v>124</v>
+      </c>
+      <c r="D254">
+        <v>300</v>
+      </c>
+      <c r="E254">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>60</v>
+      </c>
+      <c r="B255" s="10">
+        <v>2</v>
+      </c>
+      <c r="C255" t="s">
+        <v>20</v>
+      </c>
+      <c r="D255">
+        <v>300</v>
+      </c>
+      <c r="E255">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>60</v>
+      </c>
+      <c r="B256" s="10">
+        <v>2</v>
+      </c>
+      <c r="C256" t="s">
+        <v>21</v>
+      </c>
+      <c r="D256">
+        <v>300</v>
+      </c>
+      <c r="E256">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>60</v>
+      </c>
+      <c r="B257" s="10">
+        <v>2</v>
+      </c>
+      <c r="C257" t="s">
+        <v>23</v>
+      </c>
+      <c r="D257">
+        <v>300</v>
+      </c>
+      <c r="E257">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>60</v>
+      </c>
+      <c r="B258" s="10">
+        <v>2</v>
+      </c>
+      <c r="C258" t="s">
+        <v>24</v>
+      </c>
+      <c r="D258">
+        <v>300</v>
+      </c>
+      <c r="E258">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>60</v>
+      </c>
+      <c r="B259" s="10">
+        <v>2</v>
+      </c>
+      <c r="C259" t="s">
+        <v>16</v>
+      </c>
+      <c r="D259">
+        <v>198</v>
+      </c>
+      <c r="E259">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>49</v>
+      </c>
+      <c r="B260" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C260" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D260">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>62</v>
+      </c>
+      <c r="B261" s="10">
+        <v>1</v>
+      </c>
+      <c r="C261" t="s">
+        <v>127</v>
+      </c>
+      <c r="D261">
+        <v>301</v>
+      </c>
+      <c r="E261">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>63</v>
+      </c>
+      <c r="B262" s="10">
+        <v>1</v>
+      </c>
+      <c r="C262" t="s">
+        <v>127</v>
+      </c>
+      <c r="D262">
+        <v>302</v>
+      </c>
+      <c r="E262">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>63</v>
+      </c>
+      <c r="B263" s="10">
+        <v>1</v>
+      </c>
+      <c r="C263" t="s">
+        <v>127</v>
+      </c>
+      <c r="D263">
+        <v>308</v>
+      </c>
+      <c r="E263">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>63</v>
+      </c>
+      <c r="B264" s="10">
+        <v>1</v>
+      </c>
+      <c r="C264" t="s">
+        <v>127</v>
+      </c>
+      <c r="D264">
+        <v>309</v>
+      </c>
+      <c r="E264">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>73</v>
+      </c>
+      <c r="B265" s="10">
+        <v>1</v>
+      </c>
+      <c r="C265" t="s">
+        <v>127</v>
+      </c>
+      <c r="D265">
+        <v>310</v>
+      </c>
+      <c r="E265">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>74</v>
+      </c>
+      <c r="B266" s="10">
+        <v>1</v>
+      </c>
+      <c r="C266" t="s">
+        <v>127</v>
+      </c>
+      <c r="D266">
+        <v>317</v>
+      </c>
+      <c r="E266">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>75</v>
+      </c>
+      <c r="B267" s="10">
+        <v>1</v>
+      </c>
+      <c r="C267" t="s">
+        <v>111</v>
+      </c>
+      <c r="D267">
+        <v>365</v>
+      </c>
+      <c r="E267">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>75</v>
+      </c>
+      <c r="B268" s="10">
+        <v>1</v>
+      </c>
+      <c r="C268" t="s">
+        <v>111</v>
+      </c>
+      <c r="D268">
+        <v>366</v>
+      </c>
+      <c r="E268">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>75</v>
+      </c>
+      <c r="B269" s="10">
+        <v>1</v>
+      </c>
+      <c r="C269" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D269" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E269" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F269" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>76</v>
+      </c>
+      <c r="B270" s="10">
+        <v>1</v>
+      </c>
+      <c r="C270" t="s">
+        <v>130</v>
+      </c>
+      <c r="D270">
+        <v>250</v>
+      </c>
+      <c r="E270">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>76</v>
+      </c>
+      <c r="B271" s="10">
+        <v>1</v>
+      </c>
+      <c r="C271" t="s">
+        <v>25</v>
+      </c>
+      <c r="D271">
+        <v>215</v>
+      </c>
+      <c r="E271">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>77</v>
+      </c>
+      <c r="B272" s="10">
+        <v>1</v>
+      </c>
+      <c r="C272" t="s">
+        <v>131</v>
+      </c>
+      <c r="D272">
+        <v>260</v>
+      </c>
+      <c r="E272">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>78</v>
+      </c>
+      <c r="B273" s="10">
+        <v>1</v>
+      </c>
+      <c r="C273" t="s">
+        <v>132</v>
+      </c>
+      <c r="D273">
+        <v>332</v>
+      </c>
+      <c r="E273">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>89</v>
+      </c>
+      <c r="B274" s="10">
+        <v>1</v>
+      </c>
+      <c r="C274" t="s">
+        <v>127</v>
+      </c>
+      <c r="D274">
+        <v>401</v>
+      </c>
+      <c r="E274">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>96</v>
+      </c>
+      <c r="B275" s="10">
+        <v>1</v>
+      </c>
+      <c r="C275" t="s">
+        <v>25</v>
+      </c>
+      <c r="D275">
+        <v>460</v>
+      </c>
+      <c r="E275">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>96</v>
+      </c>
+      <c r="B276" s="10">
+        <v>1</v>
+      </c>
+      <c r="C276" t="s">
+        <v>129</v>
+      </c>
+      <c r="D276">
+        <v>380</v>
+      </c>
+      <c r="E276">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>96</v>
+      </c>
+      <c r="B277" s="10">
+        <v>1</v>
+      </c>
+      <c r="C277" t="s">
+        <v>133</v>
+      </c>
+      <c r="D277">
+        <v>460</v>
+      </c>
+      <c r="E277">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>97</v>
+      </c>
+      <c r="B278" s="10">
+        <v>1</v>
+      </c>
+      <c r="C278" t="s">
+        <v>127</v>
+      </c>
+      <c r="D278">
+        <v>480</v>
+      </c>
+      <c r="E278">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>59</v>
+      </c>
+      <c r="B279" s="10">
+        <v>5</v>
+      </c>
+      <c r="C279" t="s">
+        <v>127</v>
+      </c>
+      <c r="D279">
+        <v>300</v>
+      </c>
+      <c r="E279">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>59</v>
+      </c>
+      <c r="B280" s="10">
+        <v>5</v>
+      </c>
+      <c r="C280" t="s">
+        <v>136</v>
+      </c>
+      <c r="D280">
+        <v>300</v>
+      </c>
+      <c r="E280">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>59</v>
+      </c>
+      <c r="B281" s="10">
+        <v>5</v>
+      </c>
+      <c r="C281" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D281" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E281" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F281" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A109 A111:A1048576">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="elc ">
+  <conditionalFormatting sqref="A1:A137 A139:A164 A166:A176 A178:A190 A208:A232 A234:A259 A261:A1048576 A192:A206">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="elc ">
       <formula>NOT(ISERROR(SEARCH("elc ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="cor ">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="cor ">
       <formula>NOT(ISERROR(SEARCH("cor ",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="add ">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="add ">
       <formula>NOT(ISERROR(SEARCH("add ",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2852,10 +5973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AC27B8-1BF8-42B7-96D3-0055CAD9AC91}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,7 +5987,7 @@
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2879,80 +6000,153 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1">
+        <f>COUNTA(D2:D29)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2994,31 +6188,102 @@
       <c r="A24" t="s">
         <v>49</v>
       </c>
+      <c r="B24" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="B25" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="8" t="s">
         <v>52</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
+      <c r="B27" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
+      <c r="B28" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
+      <c r="B29" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -3037,19 +6302,26 @@
         <v>72</v>
       </c>
     </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A32">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="elc ">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="elc ">
       <formula>NOT(ISERROR(SEARCH("elc ",A32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="cor ">
+    <cfRule type="containsText" dxfId="1" priority="14" operator="containsText" text="cor ">
       <formula>NOT(ISERROR(SEARCH("cor ",A32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="add ">
+    <cfRule type="containsText" dxfId="0" priority="15" operator="containsText" text="add ">
       <formula>NOT(ISERROR(SEARCH("add ",A32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3565,4 +6837,192 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3301E5F-010C-4021-8BC2-3B4BCEAE84A8}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C16">
+    <sortCondition ref="C3:C16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added the codes for the main parts of the other 3 types of degree planners
</commit_message>
<xml_diff>
--- a/prerequisites/trial prereq/execution_files/majors list.xlsx
+++ b/prerequisites/trial prereq/execution_files/majors list.xlsx
@@ -1764,8 +1764,8 @@
   <dimension ref="A1:G754"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F659" sqref="F659"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H186" sqref="H186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14614,7 +14614,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="A1 A3:A35 A37:A69 A71:A109 A111:A137 A139:A164 A166:A177 A179:A190 A192:A206 A208:A232 A234:A259 A335:A406 A408:A457 A459:A482 A484:A508 A510:A532 A534:A545 A547:A560 A562:A593 A595:A629 A631:A638 A640:A651 A693:A705 A707:A720 A722:A1048576 A261:A333 A653:A691">
+  <conditionalFormatting sqref="A1 A3:A35 A37:A69 A71:A109 A111:A137 A139:A164 A166:A177 A179:A190 A192:A206 A208:A232 A234:A259 A261:A333 A335:A406 A408:A457 A459:A482 A484:A508 A510:A532 A534:A545 A547:A560 A562:A593 A595:A629 A631:A638 A640:A651 A653:A691 A693:A705 A707:A720 A722:A1048576">
     <cfRule type="containsText" dxfId="5" priority="22" operator="containsText" text="elc ">
       <formula>NOT(ISERROR(SEARCH("elc ",A1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
added the new folder structure
</commit_message>
<xml_diff>
--- a/prerequisites/trial prereq/execution_files/majors list.xlsx
+++ b/prerequisites/trial prereq/execution_files/majors list.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2695" documentId="13_ncr:1_{C33D7932-E03C-452A-ACDA-0A7400E5C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D2C2EAD-3C89-4942-833D-90D9E0EF6FCE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39B82AA1-F665-4363-970D-8821589D72FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{39B82AA1-F665-4363-970D-8821589D72FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Majors" sheetId="6" r:id="rId1"/>
@@ -1831,7 +1831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701C36C7-83AA-41D8-8B1C-C0D8358D86FD}">
   <dimension ref="A1:G822"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A191" sqref="A1:A1048576"/>
     </sheetView>
@@ -15805,8 +15805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AC27B8-1BF8-42B7-96D3-0055CAD9AC91}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>